<commit_message>
añadir a la bitacora caida de nextlab por fuente
</commit_message>
<xml_diff>
--- a/BITACORA.xlsx
+++ b/BITACORA.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bitacora\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81F7BF0E-39D4-43DB-A62F-B0932FF3238C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{89244FFE-E438-4398-ADE9-BF69DA91141B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DB689F4F-3024-4C60-A999-50832C9E29C1}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="55">
   <si>
     <t>BITACORA SISTEMAS</t>
   </si>
@@ -122,9 +122,6 @@
   </si>
   <si>
     <t>NO SE PODIAN VISUALIZAR ALGUNOS INFORMES</t>
-  </si>
-  <si>
-    <t>REINICIO DEL SERVIDOR DE APLICACIONES GLASSFISH</t>
   </si>
   <si>
     <t>INGRESAR AL SERVIDOR 4 CON TEAMVIEWER, PODEMOS ELIMINAR LOS LOGS SI ES QUE EXISTEN PREFERIBLEMENTE DE UN DIA ANTES EN EL QUE SE ENCUENTRA</t>
@@ -192,6 +189,29 @@
   </si>
   <si>
     <t>https://github.com/conejo7/bitacora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REINICIO DEL SERVIDOR DE APLICACIONES GLASSFISH
+se comprobo que solo se debe reiniciar el servidor de aplicaciones wildfly que esta el web service </t>
+  </si>
+  <si>
+    <t>N5</t>
+  </si>
+  <si>
+    <t>NO GUARDABA Y EL DE LIBERACION SE QUEDABA PENSANDO</t>
+  </si>
+  <si>
+    <t>SE REVISO LOS PROCESOS Y HABIA 200 QUE NO SE ELIMINABAN, SE LES ELIMINO 
+Y YA FUNCIONABA CORRECTAMENTE</t>
+  </si>
+  <si>
+    <t>N6</t>
+  </si>
+  <si>
+    <t>NO VISUALIZABA NADA, COMO SI ESTUVIERA en estado de hibernación</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SE LE APAGO Y SE REINICIO PORQUE NO RESPONDIA </t>
   </si>
 </sst>
 </file>
@@ -682,23 +702,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1903565A-9A1F-4BE4-B062-F63E710A5C65}">
-  <dimension ref="B4:M66"/>
+  <dimension ref="A4:M72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.21875" customWidth="1"/>
     <col min="3" max="3" width="31.6640625" customWidth="1"/>
     <col min="4" max="4" width="16.21875" customWidth="1"/>
-    <col min="5" max="5" width="47.33203125" customWidth="1"/>
+    <col min="5" max="5" width="61.109375" customWidth="1"/>
     <col min="6" max="6" width="67.33203125" customWidth="1"/>
     <col min="7" max="7" width="46.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B4" t="s">
         <v>19</v>
       </c>
@@ -707,7 +727,7 @@
       </c>
       <c r="D4" s="2"/>
     </row>
-    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B5" t="s">
         <v>20</v>
       </c>
@@ -716,7 +736,7 @@
       </c>
       <c r="D5" s="3"/>
     </row>
-    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B6" t="s">
         <v>23</v>
       </c>
@@ -725,7 +745,7 @@
       </c>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B7" t="s">
         <v>9</v>
       </c>
@@ -734,7 +754,7 @@
       </c>
       <c r="D7" s="1"/>
     </row>
-    <row r="8" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>25</v>
       </c>
@@ -743,16 +763,16 @@
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="15"/>
     </row>
-    <row r="11" spans="2:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="24" t="s">
         <v>0</v>
       </c>
@@ -768,7 +788,7 @@
       <c r="L11" s="24"/>
       <c r="M11" s="24"/>
     </row>
-    <row r="12" spans="2:13" ht="21" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" ht="21" x14ac:dyDescent="0.4">
       <c r="B12" s="6" t="s">
         <v>1</v>
       </c>
@@ -794,24 +814,27 @@
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
     </row>
-    <row r="13" spans="2:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="21">
-        <v>44214</v>
-      </c>
-      <c r="C13" s="20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D13" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="E13" s="9" t="s">
-        <v>5</v>
-      </c>
-      <c r="F13" s="9" t="s">
-        <v>6</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>12</v>
+    <row r="13" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13" s="8">
+        <v>44177</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" s="13" t="s">
+        <v>42</v>
       </c>
       <c r="H13" s="7"/>
       <c r="I13" s="7"/>
@@ -820,22 +843,27 @@
       <c r="L13" s="7"/>
       <c r="M13" s="7"/>
     </row>
-    <row r="14" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B14" s="7"/>
+    <row r="14" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>2</v>
+      </c>
+      <c r="B14" s="21">
+        <v>44214</v>
+      </c>
       <c r="C14" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="D14" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>11</v>
+      <c r="D14" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>5</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>18</v>
+        <v>6</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>12</v>
       </c>
       <c r="H14" s="7"/>
       <c r="I14" s="7"/>
@@ -844,19 +872,24 @@
       <c r="L14" s="7"/>
       <c r="M14" s="7"/>
     </row>
-    <row r="15" spans="2:13" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B15" s="7"/>
+    <row r="15" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>3</v>
+      </c>
+      <c r="B15" s="8">
+        <v>44214</v>
+      </c>
       <c r="C15" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D15" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="11" t="s">
-        <v>42</v>
+        <v>15</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="G15" s="12" t="s">
         <v>18</v>
@@ -868,13 +901,28 @@
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
     </row>
-    <row r="16" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B16" s="7"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="7"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="7"/>
+    <row r="16" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>4</v>
+      </c>
+      <c r="B16" s="8">
+        <v>44214</v>
+      </c>
+      <c r="C16" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H16" s="7"/>
       <c r="I16" s="7"/>
       <c r="J16" s="7"/>
@@ -882,24 +930,27 @@
       <c r="L16" s="7"/>
       <c r="M16" s="7"/>
     </row>
-    <row r="17" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>5</v>
+      </c>
       <c r="B17" s="8">
         <v>44214</v>
       </c>
-      <c r="C17" s="16" t="s">
-        <v>20</v>
+      <c r="C17" s="18" t="s">
+        <v>35</v>
       </c>
       <c r="D17" s="7" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="E17" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="F17" s="7" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>38</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>18</v>
+        <v>42</v>
       </c>
       <c r="H17" s="7"/>
       <c r="I17" s="7"/>
@@ -908,13 +959,28 @@
       <c r="L17" s="7"/>
       <c r="M17" s="7"/>
     </row>
-    <row r="18" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B18" s="7"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="7"/>
-      <c r="G18" s="7"/>
+    <row r="18" spans="1:13" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" s="8">
+        <v>44214</v>
+      </c>
+      <c r="C18" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="F18" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="13" t="s">
+        <v>18</v>
+      </c>
       <c r="H18" s="7"/>
       <c r="I18" s="7"/>
       <c r="J18" s="7"/>
@@ -922,21 +988,24 @@
       <c r="L18" s="7"/>
       <c r="M18" s="7"/>
     </row>
-    <row r="19" spans="2:13" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>7</v>
+      </c>
       <c r="B19" s="8">
         <v>44214</v>
       </c>
       <c r="C19" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="D19" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="D19" s="7" t="s">
+      <c r="E19" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="F19" s="7" t="s">
         <v>33</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>34</v>
       </c>
       <c r="G19" s="13" t="s">
         <v>18</v>
@@ -948,13 +1017,28 @@
       <c r="L19" s="7"/>
       <c r="M19" s="7"/>
     </row>
-    <row r="20" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B20" s="7"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="7"/>
+    <row r="20" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>9</v>
+      </c>
+      <c r="B20" s="8">
+        <v>44222</v>
+      </c>
+      <c r="C20" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G20" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H20" s="7"/>
       <c r="I20" s="7"/>
       <c r="J20" s="7"/>
@@ -962,22 +1046,27 @@
       <c r="L20" s="7"/>
       <c r="M20" s="7"/>
     </row>
-    <row r="21" spans="2:13" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B21" s="7"/>
-      <c r="C21" s="18" t="s">
-        <v>36</v>
+    <row r="21" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>10</v>
+      </c>
+      <c r="B21" s="8">
+        <v>44225</v>
+      </c>
+      <c r="C21" s="20" t="s">
+        <v>3</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>37</v>
-      </c>
-      <c r="E21" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>39</v>
-      </c>
-      <c r="G21" s="13" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="H21" s="7"/>
       <c r="I21" s="7"/>
@@ -986,13 +1075,16 @@
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
     </row>
-    <row r="22" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B22" s="7"/>
-      <c r="C22" s="7"/>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>11</v>
+      </c>
+      <c r="B22" s="8"/>
+      <c r="C22" s="20"/>
       <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
+      <c r="E22" s="11"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="12"/>
       <c r="H22" s="7"/>
       <c r="I22" s="7"/>
       <c r="J22" s="7"/>
@@ -1000,22 +1092,27 @@
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
     </row>
-    <row r="23" spans="2:13" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B23" s="7"/>
-      <c r="C23" s="19" t="s">
-        <v>23</v>
+    <row r="23" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23" s="8">
+        <v>44201</v>
+      </c>
+      <c r="C23" s="20" t="s">
+        <v>3</v>
       </c>
       <c r="D23" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="E23" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="F23" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="G23" s="13" t="s">
-        <v>43</v>
+        <v>15</v>
+      </c>
+      <c r="E23" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>18</v>
       </c>
       <c r="H23" s="7"/>
       <c r="I23" s="7"/>
@@ -1024,24 +1121,27 @@
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
     </row>
-    <row r="24" spans="2:13" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>14</v>
+      </c>
       <c r="B24" s="8">
-        <v>44246</v>
-      </c>
-      <c r="C24" s="23" t="s">
+        <v>44202</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>3</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="F24" s="11" t="s">
-        <v>47</v>
+        <v>15</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>29</v>
       </c>
       <c r="G24" s="12" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="H24" s="7"/>
       <c r="I24" s="7"/>
@@ -1050,13 +1150,28 @@
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
     </row>
-    <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="7"/>
-      <c r="F25" s="7"/>
-      <c r="G25" s="7"/>
+    <row r="25" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25" s="8">
+        <v>44204</v>
+      </c>
+      <c r="C25" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F25" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H25" s="7"/>
       <c r="I25" s="7"/>
       <c r="J25" s="7"/>
@@ -1064,13 +1179,28 @@
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
     </row>
-    <row r="26" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="7"/>
-      <c r="E26" s="7"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="7"/>
+    <row r="26" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26" s="8">
+        <v>44206</v>
+      </c>
+      <c r="C26" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G26" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H26" s="7"/>
       <c r="I26" s="7"/>
       <c r="J26" s="7"/>
@@ -1078,13 +1208,28 @@
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
     </row>
-    <row r="27" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="7"/>
+    <row r="27" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>17</v>
+      </c>
+      <c r="B27" s="8">
+        <v>44210</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G27" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H27" s="7"/>
       <c r="I27" s="7"/>
       <c r="J27" s="7"/>
@@ -1092,13 +1237,28 @@
       <c r="L27" s="7"/>
       <c r="M27" s="7"/>
     </row>
-    <row r="28" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B28" s="7"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="7"/>
-      <c r="E28" s="7"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="7"/>
+    <row r="28" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>18</v>
+      </c>
+      <c r="B28" s="8">
+        <v>44211</v>
+      </c>
+      <c r="C28" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E28" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G28" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H28" s="7"/>
       <c r="I28" s="7"/>
       <c r="J28" s="7"/>
@@ -1106,13 +1266,28 @@
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
     </row>
-    <row r="29" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="7"/>
-      <c r="E29" s="7"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="7"/>
+    <row r="29" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>19</v>
+      </c>
+      <c r="B29" s="8">
+        <v>44245</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="12" t="s">
+        <v>18</v>
+      </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -1120,13 +1295,28 @@
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
     </row>
-    <row r="30" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="7"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="7"/>
-      <c r="G30" s="7"/>
+    <row r="30" spans="1:13" ht="111" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>20</v>
+      </c>
+      <c r="B30" s="8">
+        <v>44246</v>
+      </c>
+      <c r="C30" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E30" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="G30" s="12" t="s">
+        <v>47</v>
+      </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7"/>
       <c r="J30" s="7"/>
@@ -1134,13 +1324,25 @@
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
     </row>
-    <row r="31" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B31" s="7"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="7"/>
-      <c r="E31" s="7"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="7"/>
+    <row r="31" spans="1:13" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B31" s="8">
+        <v>44249</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D31" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>47</v>
+      </c>
       <c r="H31" s="7"/>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -1148,12 +1350,22 @@
       <c r="L31" s="7"/>
       <c r="M31" s="7"/>
     </row>
-    <row r="32" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B32" s="7"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="7"/>
-      <c r="E32" s="7"/>
-      <c r="F32" s="7"/>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B32" s="8">
+        <v>44258</v>
+      </c>
+      <c r="C32" s="23" t="s">
+        <v>3</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="F32" s="7" t="s">
+        <v>54</v>
+      </c>
       <c r="G32" s="7"/>
       <c r="H32" s="7"/>
       <c r="I32" s="7"/>
@@ -1638,21 +1850,114 @@
       <c r="L66" s="7"/>
       <c r="M66" s="7"/>
     </row>
+    <row r="67" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="7"/>
+      <c r="E67" s="7"/>
+      <c r="F67" s="7"/>
+      <c r="G67" s="7"/>
+      <c r="H67" s="7"/>
+      <c r="I67" s="7"/>
+      <c r="J67" s="7"/>
+      <c r="K67" s="7"/>
+      <c r="L67" s="7"/>
+      <c r="M67" s="7"/>
+    </row>
+    <row r="68" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B68" s="7"/>
+      <c r="C68" s="7"/>
+      <c r="D68" s="7"/>
+      <c r="E68" s="7"/>
+      <c r="F68" s="7"/>
+      <c r="G68" s="7"/>
+      <c r="H68" s="7"/>
+      <c r="I68" s="7"/>
+      <c r="J68" s="7"/>
+      <c r="K68" s="7"/>
+      <c r="L68" s="7"/>
+      <c r="M68" s="7"/>
+    </row>
+    <row r="69" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B69" s="7"/>
+      <c r="C69" s="7"/>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7"/>
+      <c r="G69" s="7"/>
+      <c r="H69" s="7"/>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="7"/>
+    </row>
+    <row r="70" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="7"/>
+      <c r="E70" s="7"/>
+      <c r="F70" s="7"/>
+      <c r="G70" s="7"/>
+      <c r="H70" s="7"/>
+      <c r="I70" s="7"/>
+      <c r="J70" s="7"/>
+      <c r="K70" s="7"/>
+      <c r="L70" s="7"/>
+      <c r="M70" s="7"/>
+    </row>
+    <row r="71" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="7"/>
+      <c r="E71" s="7"/>
+      <c r="F71" s="7"/>
+      <c r="G71" s="7"/>
+      <c r="H71" s="7"/>
+      <c r="I71" s="7"/>
+      <c r="J71" s="7"/>
+      <c r="K71" s="7"/>
+      <c r="L71" s="7"/>
+      <c r="M71" s="7"/>
+    </row>
+    <row r="72" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="7"/>
+      <c r="E72" s="7"/>
+      <c r="F72" s="7"/>
+      <c r="G72" s="7"/>
+      <c r="H72" s="7"/>
+      <c r="I72" s="7"/>
+      <c r="J72" s="7"/>
+      <c r="K72" s="7"/>
+      <c r="L72" s="7"/>
+      <c r="M72" s="7"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B11:M11"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="G13" r:id="rId1" display="https://github.com/conejo7/bitacora.git" xr:uid="{E66C1F00-79BD-43C3-8C3E-BBBD82F2DF1F}"/>
-    <hyperlink ref="G14" r:id="rId2" display="https://github.com/conejo7/bitacora" xr:uid="{C6478953-FC6B-4492-82D3-FC7AF9C5AF7B}"/>
-    <hyperlink ref="G15" r:id="rId3" display="https://github.com/conejo7/bitacora" xr:uid="{35684D8C-5BA0-41BF-A28D-2F8C057848BA}"/>
-    <hyperlink ref="G17" r:id="rId4" display="https://github.com/conejo7/bitacora" xr:uid="{E759EC94-8FC5-42E9-9644-41AB6A7A5185}"/>
+    <hyperlink ref="G14" r:id="rId1" display="https://github.com/conejo7/bitacora.git" xr:uid="{E66C1F00-79BD-43C3-8C3E-BBBD82F2DF1F}"/>
+    <hyperlink ref="G15" r:id="rId2" display="https://github.com/conejo7/bitacora" xr:uid="{C6478953-FC6B-4492-82D3-FC7AF9C5AF7B}"/>
+    <hyperlink ref="G16" r:id="rId3" display="https://github.com/conejo7/bitacora" xr:uid="{35684D8C-5BA0-41BF-A28D-2F8C057848BA}"/>
+    <hyperlink ref="G18" r:id="rId4" display="https://github.com/conejo7/bitacora" xr:uid="{E759EC94-8FC5-42E9-9644-41AB6A7A5185}"/>
     <hyperlink ref="G19" r:id="rId5" display="https://github.com/conejo7/bitacora" xr:uid="{1EE8F3D9-4A66-4D83-8F7B-E2E112ABBF43}"/>
-    <hyperlink ref="G21" r:id="rId6" display="https://github.com/conejo7/bitacora" xr:uid="{07747805-E213-4CCE-805C-9C972BE47D88}"/>
-    <hyperlink ref="G23" r:id="rId7" display="https://github.com/conejo7/bitacora" xr:uid="{8C1F9F97-0EBD-433F-86E9-1771A3047CF8}"/>
-    <hyperlink ref="G24" r:id="rId8" xr:uid="{02F73619-97B2-435B-B0DC-7111C165433B}"/>
+    <hyperlink ref="G17" r:id="rId6" display="https://github.com/conejo7/bitacora" xr:uid="{07747805-E213-4CCE-805C-9C972BE47D88}"/>
+    <hyperlink ref="G13" r:id="rId7" display="https://github.com/conejo7/bitacora" xr:uid="{8C1F9F97-0EBD-433F-86E9-1771A3047CF8}"/>
+    <hyperlink ref="G30" r:id="rId8" xr:uid="{02F73619-97B2-435B-B0DC-7111C165433B}"/>
+    <hyperlink ref="G29" r:id="rId9" display="https://github.com/conejo7/bitacora" xr:uid="{C9499137-9165-4C0D-9765-7EE0C9803B1E}"/>
+    <hyperlink ref="G28" r:id="rId10" display="https://github.com/conejo7/bitacora" xr:uid="{99F79797-8BC4-486F-A508-31942794FCEA}"/>
+    <hyperlink ref="G25" r:id="rId11" display="https://github.com/conejo7/bitacora" xr:uid="{D8B77E70-9DE2-4BD5-B120-3F5B17726BC6}"/>
+    <hyperlink ref="G26" r:id="rId12" display="https://github.com/conejo7/bitacora" xr:uid="{A332290E-3E26-4122-AE01-26320D9DE2EA}"/>
+    <hyperlink ref="G27" r:id="rId13" display="https://github.com/conejo7/bitacora" xr:uid="{2C3AF4AC-7CBC-49E5-A6F4-4C60022DC0D2}"/>
+    <hyperlink ref="G24" r:id="rId14" display="https://github.com/conejo7/bitacora" xr:uid="{5A399172-3BF8-4F83-A144-E9387FB5E3A2}"/>
+    <hyperlink ref="G21" r:id="rId15" display="https://github.com/conejo7/bitacora" xr:uid="{0C40215B-B451-4114-B910-5F5F3C2E7255}"/>
+    <hyperlink ref="G20" r:id="rId16" display="https://github.com/conejo7/bitacora" xr:uid="{7E91F7DD-F3D4-4AF4-AA9A-336E52A346D5}"/>
+    <hyperlink ref="G23" r:id="rId17" display="https://github.com/conejo7/bitacora" xr:uid="{9D5EDF45-8512-4727-B982-ECD724625477}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId9"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId18"/>
 </worksheet>
 </file>
</xml_diff>